<commit_message>
removed 2 machines and put the file uploading in Horiba
</commit_message>
<xml_diff>
--- a/linked_data.xlsx
+++ b/linked_data.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -422,852 +434,852 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>profile_id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>profile_found</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>school</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>class</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>section</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>horiba</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>submitted_at</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>response_id</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>age</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>age_completed</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>anemia_status</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>birth_order</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>capillary_attempts</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>capillary_hb_value</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>caste_category</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>child_classification</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>child_id_code</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>child_response_score</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>chronic_illness</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>chronic_illness_history</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>chronic_illness_specify</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>comfortable_testing_process</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>device_sequence</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>deworming_history</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>deworming_tablet</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>diet_type</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>district</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>dob</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>edu_head_family</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>edu_head_level</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>edu_score</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>extra_54</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>extra_55</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>family_income_level</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>family_members_count</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>family_members_total</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>family_type</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>freq_dates</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>freq_eggs</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>freq_fruits</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>freq_green_leafy</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>freq_jaggery</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>freq_meat</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>gender</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>hb_measurement_datetime</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>height_cm</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>hemocue</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>ifa_dose</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>income_score</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>investigator_entry_note</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>investigator_name</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>investigator_signature</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>investigator_username</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>iron_rich_food_frequency</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>iron_supplementation</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>iron_supplementation_current</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>kupp_total_score</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>kuppuswamy_total_score</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>lab_attempts</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>lab_calibration</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>lab_ease</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>lab_end_time</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>lab_flacc_activity</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
+          <t>lab_flacc_consolability</t>
+        </is>
+      </c>
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
+          <t>lab_flacc_cry</t>
+        </is>
+      </c>
+      <c r="BO1" s="1" t="inlineStr">
+        <is>
+          <t>lab_flacc_face</t>
+        </is>
+      </c>
+      <c r="BP1" s="1" t="inlineStr">
+        <is>
+          <t>lab_flacc_legs</t>
+        </is>
+      </c>
+      <c r="BQ1" s="1" t="inlineStr">
+        <is>
+          <t>lab_flacc_total</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>lab_hb_value</t>
+        </is>
+      </c>
+      <c r="BS1" s="1" t="inlineStr">
+        <is>
+          <t>lab_maintenance</t>
+        </is>
+      </c>
+      <c r="BT1" s="1" t="inlineStr">
+        <is>
+          <t>lab_portability</t>
+        </is>
+      </c>
+      <c r="BU1" s="1" t="inlineStr">
+        <is>
+          <t>lab_practicality</t>
+        </is>
+      </c>
+      <c r="BV1" s="1" t="inlineStr">
+        <is>
+          <t>lab_recording</t>
+        </is>
+      </c>
+      <c r="BW1" s="1" t="inlineStr">
+        <is>
+          <t>lab_reliability</t>
+        </is>
+      </c>
+      <c r="BX1" s="1" t="inlineStr">
+        <is>
+          <t>lab_safety</t>
+        </is>
+      </c>
+      <c r="BY1" s="1" t="inlineStr">
+        <is>
+          <t>lab_start_time</t>
+        </is>
+      </c>
+      <c r="BZ1" s="1" t="inlineStr">
+        <is>
+          <t>lab_suitability</t>
+        </is>
+      </c>
+      <c r="CA1" s="1" t="inlineStr">
+        <is>
+          <t>lab_training</t>
+        </is>
+      </c>
+      <c r="CB1" s="1" t="inlineStr">
+        <is>
+          <t>linked_at</t>
+        </is>
+      </c>
+      <c r="CC1" s="1" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
+      <c r="CD1" s="1" t="inlineStr">
+        <is>
+          <t>location_type</t>
+        </is>
+      </c>
+      <c r="CE1" s="1" t="inlineStr">
+        <is>
+          <t>low_birth_weight</t>
+        </is>
+      </c>
+      <c r="CF1" s="1" t="inlineStr">
+        <is>
+          <t>low_birth_weight_history</t>
+        </is>
+      </c>
+      <c r="CG1" s="1" t="inlineStr">
         <is>
           <t>masimo</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>hemocue</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>horiba</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>submitted_at</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>response_id</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>age</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>age_completed</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>anemia_status</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>birth_order</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>capillary_attempts</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>capillary_hb_value</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>caste_category</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>child_classification</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>child_id_code</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>child_response_score</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>chronic_illness</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>chronic_illness_history</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>chronic_illness_specify</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>comfortable_testing_process</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>device_sequence</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>deworming_history</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>deworming_tablet</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>diet_type</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>district</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>dob</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>edu_head_family</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>edu_head_level</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>edu_score</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>extra_54</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>extra_55</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>family_income_level</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>family_members_count</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>family_members_total</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>family_type</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>freq_dates</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>freq_eggs</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>freq_fruits</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>freq_green_leafy</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>freq_jaggery</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>freq_meat</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>gender</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>hb_measurement_datetime</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>height_cm</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>ifa_dose</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>income_score</t>
-        </is>
-      </c>
-      <c r="AZ1" t="inlineStr">
-        <is>
-          <t>investigator_entry_note</t>
-        </is>
-      </c>
-      <c r="BA1" t="inlineStr">
-        <is>
-          <t>investigator_name</t>
-        </is>
-      </c>
-      <c r="BB1" t="inlineStr">
-        <is>
-          <t>investigator_signature</t>
-        </is>
-      </c>
-      <c r="BC1" t="inlineStr">
-        <is>
-          <t>investigator_username</t>
-        </is>
-      </c>
-      <c r="BD1" t="inlineStr">
-        <is>
-          <t>iron_rich_food_frequency</t>
-        </is>
-      </c>
-      <c r="BE1" t="inlineStr">
-        <is>
-          <t>iron_supplementation</t>
-        </is>
-      </c>
-      <c r="BF1" t="inlineStr">
-        <is>
-          <t>iron_supplementation_current</t>
-        </is>
-      </c>
-      <c r="BG1" t="inlineStr">
-        <is>
-          <t>kupp_total_score</t>
-        </is>
-      </c>
-      <c r="BH1" t="inlineStr">
-        <is>
-          <t>kuppuswamy_total_score</t>
-        </is>
-      </c>
-      <c r="BI1" t="inlineStr">
-        <is>
-          <t>lab_attempts</t>
-        </is>
-      </c>
-      <c r="BJ1" t="inlineStr">
-        <is>
-          <t>lab_calibration</t>
-        </is>
-      </c>
-      <c r="BK1" t="inlineStr">
-        <is>
-          <t>lab_ease</t>
-        </is>
-      </c>
-      <c r="BL1" t="inlineStr">
-        <is>
-          <t>lab_end_time</t>
-        </is>
-      </c>
-      <c r="BM1" t="inlineStr">
-        <is>
-          <t>lab_flacc_activity</t>
-        </is>
-      </c>
-      <c r="BN1" t="inlineStr">
-        <is>
-          <t>lab_flacc_consolability</t>
-        </is>
-      </c>
-      <c r="BO1" t="inlineStr">
-        <is>
-          <t>lab_flacc_cry</t>
-        </is>
-      </c>
-      <c r="BP1" t="inlineStr">
-        <is>
-          <t>lab_flacc_face</t>
-        </is>
-      </c>
-      <c r="BQ1" t="inlineStr">
-        <is>
-          <t>lab_flacc_legs</t>
-        </is>
-      </c>
-      <c r="BR1" t="inlineStr">
-        <is>
-          <t>lab_flacc_total</t>
-        </is>
-      </c>
-      <c r="BS1" t="inlineStr">
-        <is>
-          <t>lab_hb_value</t>
-        </is>
-      </c>
-      <c r="BT1" t="inlineStr">
-        <is>
-          <t>lab_maintenance</t>
-        </is>
-      </c>
-      <c r="BU1" t="inlineStr">
-        <is>
-          <t>lab_portability</t>
-        </is>
-      </c>
-      <c r="BV1" t="inlineStr">
-        <is>
-          <t>lab_practicality</t>
-        </is>
-      </c>
-      <c r="BW1" t="inlineStr">
-        <is>
-          <t>lab_recording</t>
-        </is>
-      </c>
-      <c r="BX1" t="inlineStr">
-        <is>
-          <t>lab_reliability</t>
-        </is>
-      </c>
-      <c r="BY1" t="inlineStr">
-        <is>
-          <t>lab_safety</t>
-        </is>
-      </c>
-      <c r="BZ1" t="inlineStr">
-        <is>
-          <t>lab_start_time</t>
-        </is>
-      </c>
-      <c r="CA1" t="inlineStr">
-        <is>
-          <t>lab_suitability</t>
-        </is>
-      </c>
-      <c r="CB1" t="inlineStr">
-        <is>
-          <t>lab_training</t>
-        </is>
-      </c>
-      <c r="CC1" t="inlineStr">
-        <is>
-          <t>linked_at</t>
-        </is>
-      </c>
-      <c r="CD1" t="inlineStr">
-        <is>
-          <t>location</t>
-        </is>
-      </c>
-      <c r="CE1" t="inlineStr">
-        <is>
-          <t>location_type</t>
-        </is>
-      </c>
-      <c r="CF1" t="inlineStr">
-        <is>
-          <t>low_birth_weight</t>
-        </is>
-      </c>
-      <c r="CG1" t="inlineStr">
-        <is>
-          <t>low_birth_weight_history</t>
-        </is>
-      </c>
-      <c r="CH1" t="inlineStr">
+      <c r="CH1" s="1" t="inlineStr">
         <is>
           <t>masimo_avg_sphb</t>
         </is>
       </c>
-      <c r="CI1" t="inlineStr">
+      <c r="CI1" s="1" t="inlineStr">
         <is>
           <t>masimo_calibration</t>
         </is>
       </c>
-      <c r="CJ1" t="inlineStr">
+      <c r="CJ1" s="1" t="inlineStr">
         <is>
           <t>masimo_ease</t>
         </is>
       </c>
-      <c r="CK1" t="inlineStr">
+      <c r="CK1" s="1" t="inlineStr">
         <is>
           <t>masimo_end_time</t>
         </is>
       </c>
-      <c r="CL1" t="inlineStr">
+      <c r="CL1" s="1" t="inlineStr">
         <is>
           <t>masimo_feasibility_rating</t>
         </is>
       </c>
-      <c r="CM1" t="inlineStr">
+      <c r="CM1" s="1" t="inlineStr">
         <is>
           <t>masimo_flacc_activity</t>
         </is>
       </c>
-      <c r="CN1" t="inlineStr">
+      <c r="CN1" s="1" t="inlineStr">
         <is>
           <t>masimo_flacc_consolability</t>
         </is>
       </c>
-      <c r="CO1" t="inlineStr">
+      <c r="CO1" s="1" t="inlineStr">
         <is>
           <t>masimo_flacc_cry</t>
         </is>
       </c>
-      <c r="CP1" t="inlineStr">
+      <c r="CP1" s="1" t="inlineStr">
         <is>
           <t>masimo_flacc_face</t>
         </is>
       </c>
-      <c r="CQ1" t="inlineStr">
+      <c r="CQ1" s="1" t="inlineStr">
         <is>
           <t>masimo_flacc_legs</t>
         </is>
       </c>
-      <c r="CR1" t="inlineStr">
+      <c r="CR1" s="1" t="inlineStr">
         <is>
           <t>masimo_flacc_total</t>
         </is>
       </c>
-      <c r="CS1" t="inlineStr">
+      <c r="CS1" s="1" t="inlineStr">
         <is>
           <t>masimo_maintenance</t>
         </is>
       </c>
-      <c r="CT1" t="inlineStr">
+      <c r="CT1" s="1" t="inlineStr">
         <is>
           <t>masimo_portability</t>
         </is>
       </c>
-      <c r="CU1" t="inlineStr">
+      <c r="CU1" s="1" t="inlineStr">
         <is>
           <t>masimo_practicality</t>
         </is>
       </c>
-      <c r="CV1" t="inlineStr">
+      <c r="CV1" s="1" t="inlineStr">
         <is>
           <t>masimo_reading</t>
         </is>
       </c>
-      <c r="CW1" t="inlineStr">
+      <c r="CW1" s="1" t="inlineStr">
         <is>
           <t>masimo_reading_1</t>
         </is>
       </c>
-      <c r="CX1" t="inlineStr">
+      <c r="CX1" s="1" t="inlineStr">
         <is>
           <t>masimo_reading_2</t>
         </is>
       </c>
-      <c r="CY1" t="inlineStr">
+      <c r="CY1" s="1" t="inlineStr">
         <is>
           <t>masimo_reading_3</t>
         </is>
       </c>
-      <c r="CZ1" t="inlineStr">
+      <c r="CZ1" s="1" t="inlineStr">
         <is>
           <t>masimo_recording</t>
         </is>
       </c>
-      <c r="DA1" t="inlineStr">
+      <c r="DA1" s="1" t="inlineStr">
         <is>
           <t>masimo_reliability</t>
         </is>
       </c>
-      <c r="DB1" t="inlineStr">
+      <c r="DB1" s="1" t="inlineStr">
         <is>
           <t>masimo_safety</t>
         </is>
       </c>
-      <c r="DC1" t="inlineStr">
+      <c r="DC1" s="1" t="inlineStr">
         <is>
           <t>masimo_start_time</t>
         </is>
       </c>
-      <c r="DD1" t="inlineStr">
+      <c r="DD1" s="1" t="inlineStr">
         <is>
           <t>masimo_suitability</t>
         </is>
       </c>
-      <c r="DE1" t="inlineStr">
+      <c r="DE1" s="1" t="inlineStr">
         <is>
           <t>masimo_training</t>
         </is>
       </c>
-      <c r="DF1" t="inlineStr">
+      <c r="DF1" s="1" t="inlineStr">
         <is>
           <t>measurement_device_sequence</t>
         </is>
       </c>
-      <c r="DG1" t="inlineStr">
+      <c r="DG1" s="1" t="inlineStr">
         <is>
           <t>mobile_no</t>
         </is>
       </c>
-      <c r="DH1" t="inlineStr">
+      <c r="DH1" s="1" t="inlineStr">
         <is>
           <t>monthly_income</t>
         </is>
       </c>
-      <c r="DI1" t="inlineStr">
+      <c r="DI1" s="1" t="inlineStr">
         <is>
           <t>occ_head_level</t>
         </is>
       </c>
-      <c r="DJ1" t="inlineStr">
+      <c r="DJ1" s="1" t="inlineStr">
         <is>
           <t>occupation_head_family</t>
         </is>
       </c>
-      <c r="DK1" t="inlineStr">
+      <c r="DK1" s="1" t="inlineStr">
         <is>
           <t>occupation_score</t>
         </is>
       </c>
-      <c r="DL1" t="inlineStr">
+      <c r="DL1" s="1" t="inlineStr">
         <is>
           <t>parent_child_calm</t>
         </is>
       </c>
-      <c r="DM1" t="inlineStr">
+      <c r="DM1" s="1" t="inlineStr">
         <is>
           <t>parent_child_distress</t>
         </is>
       </c>
-      <c r="DN1" t="inlineStr">
+      <c r="DN1" s="1" t="inlineStr">
         <is>
           <t>parent_comfort</t>
         </is>
       </c>
-      <c r="DO1" t="inlineStr">
+      <c r="DO1" s="1" t="inlineStr">
         <is>
           <t>parent_test_safety</t>
         </is>
       </c>
-      <c r="DP1" t="inlineStr">
+      <c r="DP1" s="1" t="inlineStr">
         <is>
           <t>parent_total</t>
         </is>
       </c>
-      <c r="DQ1" t="inlineStr">
+      <c r="DQ1" s="1" t="inlineStr">
         <is>
           <t>parent_trust_result</t>
         </is>
       </c>
-      <c r="DR1" t="inlineStr">
+      <c r="DR1" s="1" t="inlineStr">
         <is>
           <t>participant_name</t>
         </is>
       </c>
-      <c r="DS1" t="inlineStr">
+      <c r="DS1" s="1" t="inlineStr">
         <is>
           <t>poc_attempts</t>
         </is>
       </c>
-      <c r="DT1" t="inlineStr">
+      <c r="DT1" s="1" t="inlineStr">
         <is>
           <t>poc_calibration</t>
         </is>
       </c>
-      <c r="DU1" t="inlineStr">
+      <c r="DU1" s="1" t="inlineStr">
         <is>
           <t>poc_ease</t>
         </is>
       </c>
-      <c r="DV1" t="inlineStr">
+      <c r="DV1" s="1" t="inlineStr">
         <is>
           <t>poc_end_time</t>
         </is>
       </c>
-      <c r="DW1" t="inlineStr">
+      <c r="DW1" s="1" t="inlineStr">
         <is>
           <t>poc_feasibility_rating</t>
         </is>
       </c>
-      <c r="DX1" t="inlineStr">
+      <c r="DX1" s="1" t="inlineStr">
         <is>
           <t>poc_flacc_activity</t>
         </is>
       </c>
-      <c r="DY1" t="inlineStr">
+      <c r="DY1" s="1" t="inlineStr">
         <is>
           <t>poc_flacc_consolability</t>
         </is>
       </c>
-      <c r="DZ1" t="inlineStr">
+      <c r="DZ1" s="1" t="inlineStr">
         <is>
           <t>poc_flacc_cry</t>
         </is>
       </c>
-      <c r="EA1" t="inlineStr">
+      <c r="EA1" s="1" t="inlineStr">
         <is>
           <t>poc_flacc_face</t>
         </is>
       </c>
-      <c r="EB1" t="inlineStr">
+      <c r="EB1" s="1" t="inlineStr">
         <is>
           <t>poc_flacc_legs</t>
         </is>
       </c>
-      <c r="EC1" t="inlineStr">
+      <c r="EC1" s="1" t="inlineStr">
         <is>
           <t>poc_flacc_total</t>
         </is>
       </c>
-      <c r="ED1" t="inlineStr">
+      <c r="ED1" s="1" t="inlineStr">
         <is>
           <t>poc_hb_value</t>
         </is>
       </c>
-      <c r="EE1" t="inlineStr">
+      <c r="EE1" s="1" t="inlineStr">
         <is>
           <t>poc_maintenance</t>
         </is>
       </c>
-      <c r="EF1" t="inlineStr">
+      <c r="EF1" s="1" t="inlineStr">
         <is>
           <t>poc_portability</t>
         </is>
       </c>
-      <c r="EG1" t="inlineStr">
+      <c r="EG1" s="1" t="inlineStr">
         <is>
           <t>poc_practicality</t>
         </is>
       </c>
-      <c r="EH1" t="inlineStr">
+      <c r="EH1" s="1" t="inlineStr">
         <is>
           <t>poc_recording</t>
         </is>
       </c>
-      <c r="EI1" t="inlineStr">
+      <c r="EI1" s="1" t="inlineStr">
         <is>
           <t>poc_reliability</t>
         </is>
       </c>
-      <c r="EJ1" t="inlineStr">
+      <c r="EJ1" s="1" t="inlineStr">
         <is>
           <t>poc_safety</t>
         </is>
       </c>
-      <c r="EK1" t="inlineStr">
+      <c r="EK1" s="1" t="inlineStr">
         <is>
           <t>poc_start_time</t>
         </is>
       </c>
-      <c r="EL1" t="inlineStr">
+      <c r="EL1" s="1" t="inlineStr">
         <is>
           <t>poc_suitability</t>
         </is>
       </c>
-      <c r="EM1" t="inlineStr">
+      <c r="EM1" s="1" t="inlineStr">
         <is>
           <t>poc_training</t>
         </is>
       </c>
-      <c r="EN1" t="inlineStr">
+      <c r="EN1" s="1" t="inlineStr">
         <is>
           <t>preferred_method</t>
         </is>
       </c>
-      <c r="EO1" t="inlineStr">
+      <c r="EO1" s="1" t="inlineStr">
         <is>
           <t>previous_hb_device</t>
         </is>
       </c>
-      <c r="EP1" t="inlineStr">
+      <c r="EP1" s="1" t="inlineStr">
         <is>
           <t>previous_hb_device_other</t>
         </is>
       </c>
-      <c r="EQ1" t="inlineStr">
+      <c r="EQ1" s="1" t="inlineStr">
         <is>
           <t>previous_hb_result</t>
         </is>
       </c>
-      <c r="ER1" t="inlineStr">
+      <c r="ER1" s="1" t="inlineStr">
         <is>
           <t>previous_hb_tested</t>
         </is>
       </c>
-      <c r="ES1" t="inlineStr">
+      <c r="ES1" s="1" t="inlineStr">
         <is>
           <t>profile_id_code</t>
         </is>
       </c>
-      <c r="ET1" t="inlineStr">
+      <c r="ET1" s="1" t="inlineStr">
         <is>
           <t>profile_id_display</t>
         </is>
       </c>
-      <c r="EU1" t="inlineStr">
+      <c r="EU1" s="1" t="inlineStr">
         <is>
           <t>referral_advised</t>
         </is>
       </c>
-      <c r="EV1" t="inlineStr">
+      <c r="EV1" s="1" t="inlineStr">
         <is>
           <t>referral_date</t>
         </is>
       </c>
-      <c r="EW1" t="inlineStr">
+      <c r="EW1" s="1" t="inlineStr">
         <is>
           <t>referral_destination</t>
         </is>
       </c>
-      <c r="EX1" t="inlineStr">
+      <c r="EX1" s="1" t="inlineStr">
         <is>
           <t>referral_other_specify</t>
         </is>
       </c>
-      <c r="EY1" t="inlineStr">
+      <c r="EY1" s="1" t="inlineStr">
         <is>
           <t>religion</t>
         </is>
       </c>
-      <c r="EZ1" t="inlineStr">
+      <c r="EZ1" s="1" t="inlineStr">
         <is>
           <t>repeat_screening</t>
         </is>
       </c>
-      <c r="FA1" t="inlineStr">
+      <c r="FA1" s="1" t="inlineStr">
         <is>
           <t>school_anganwadi</t>
         </is>
       </c>
-      <c r="FB1" t="inlineStr">
+      <c r="FB1" s="1" t="inlineStr">
         <is>
           <t>school_anganwadi_name</t>
         </is>
       </c>
-      <c r="FC1" t="inlineStr">
+      <c r="FC1" s="1" t="inlineStr">
         <is>
           <t>ses_class</t>
         </is>
       </c>
-      <c r="FD1" t="inlineStr">
+      <c r="FD1" s="1" t="inlineStr">
         <is>
           <t>ses_class_label</t>
         </is>
       </c>
-      <c r="FE1" t="inlineStr">
+      <c r="FE1" s="1" t="inlineStr">
         <is>
           <t>sex</t>
         </is>
       </c>
-      <c r="FF1" t="inlineStr">
+      <c r="FF1" s="1" t="inlineStr">
         <is>
           <t>siblings_count</t>
         </is>
       </c>
-      <c r="FG1" t="inlineStr">
+      <c r="FG1" s="1" t="inlineStr">
         <is>
           <t>social_category</t>
         </is>
       </c>
-      <c r="FH1" t="inlineStr">
+      <c r="FH1" s="1" t="inlineStr">
         <is>
           <t>state</t>
         </is>
       </c>
-      <c r="FI1" t="inlineStr">
+      <c r="FI1" s="1" t="inlineStr">
         <is>
           <t>study_date</t>
         </is>
       </c>
-      <c r="FJ1" t="inlineStr">
+      <c r="FJ1" s="1" t="inlineStr">
         <is>
           <t>study_id</t>
         </is>
       </c>
-      <c r="FK1" t="inlineStr">
+      <c r="FK1" s="1" t="inlineStr">
         <is>
           <t>venous_hb_value</t>
         </is>
       </c>
-      <c r="FL1" t="inlineStr">
+      <c r="FL1" s="1" t="inlineStr">
         <is>
           <t>weight_kg</t>
         </is>
       </c>
-      <c r="FM1" t="inlineStr">
+      <c r="FM1" s="1" t="inlineStr">
         <is>
           <t>worm_infestation</t>
         </is>
       </c>
-      <c r="FN1" t="inlineStr">
+      <c r="FN1" s="1" t="inlineStr">
         <is>
           <t>worm_infestation_history</t>
         </is>
@@ -1301,27 +1313,23 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>12.8</v>
-      </c>
-      <c r="H2" t="n">
-        <v>12.4</v>
-      </c>
-      <c r="I2" t="n">
         <v>9.5</v>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>2026-02-23 05:27:05</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>15b85c3a-132e-41c1-a872-defa7708153d</t>
         </is>
       </c>
-      <c r="L2" t="n">
+      <c r="J2" t="n">
         <v>3</v>
       </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
@@ -1354,14 +1362,16 @@
       <c r="AP2" t="inlineStr"/>
       <c r="AQ2" t="inlineStr"/>
       <c r="AR2" t="inlineStr"/>
-      <c r="AS2" t="inlineStr"/>
+      <c r="AS2" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
       <c r="AT2" t="inlineStr"/>
-      <c r="AU2" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="AV2" t="inlineStr"/>
+      <c r="AU2" t="inlineStr"/>
+      <c r="AV2" t="n">
+        <v>12.4</v>
+      </c>
       <c r="AW2" t="inlineStr"/>
       <c r="AX2" t="inlineStr"/>
       <c r="AY2" t="inlineStr"/>
@@ -1398,7 +1408,9 @@
       <c r="CD2" t="inlineStr"/>
       <c r="CE2" t="inlineStr"/>
       <c r="CF2" t="inlineStr"/>
-      <c r="CG2" t="inlineStr"/>
+      <c r="CG2" t="n">
+        <v>12.8</v>
+      </c>
       <c r="CH2" t="inlineStr"/>
       <c r="CI2" t="inlineStr"/>
       <c r="CJ2" t="inlineStr"/>
@@ -1513,41 +1525,37 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>12.1</v>
-      </c>
-      <c r="H3" t="n">
-        <v>9.9</v>
-      </c>
-      <c r="I3" t="n">
         <v>5.2</v>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>2026-02-23 05:27:05</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>26cc20f0-4d91-4860-88f5-c659d7e8cd93</t>
         </is>
       </c>
-      <c r="L3" t="n">
+      <c r="J3" t="n">
         <v>2</v>
       </c>
+      <c r="K3" t="n">
+        <v>3</v>
+      </c>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N3" t="inlineStr"/>
-      <c r="O3" t="n">
-        <v>2</v>
-      </c>
-      <c r="P3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
       <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
+      <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
@@ -1557,62 +1565,64 @@
       <c r="Y3" t="inlineStr"/>
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>hyderabad</t>
+        </is>
+      </c>
       <c r="AC3" t="inlineStr"/>
       <c r="AD3" t="inlineStr">
         <is>
-          <t>hyderabad</t>
+          <t>Profession / Honours (Score 7)</t>
         </is>
       </c>
       <c r="AE3" t="inlineStr"/>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>Profession / Honours (Score 7)</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr"/>
-      <c r="AH3" t="inlineStr"/>
-      <c r="AI3" t="inlineStr">
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr">
         <is>
           <t>RACI0002</t>
         </is>
       </c>
-      <c r="AJ3" t="inlineStr">
+      <c r="AH3" t="inlineStr">
         <is>
           <t>2026-02-10 17:13:05</t>
         </is>
       </c>
-      <c r="AK3" t="inlineStr"/>
-      <c r="AL3" t="inlineStr"/>
-      <c r="AM3" t="n">
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr"/>
+      <c r="AK3" t="n">
         <v>12</v>
       </c>
-      <c r="AN3" t="inlineStr">
+      <c r="AL3" t="inlineStr">
         <is>
           <t>Nuclear</t>
         </is>
       </c>
+      <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
       <c r="AO3" t="inlineStr"/>
       <c r="AP3" t="inlineStr"/>
       <c r="AQ3" t="inlineStr"/>
       <c r="AR3" t="inlineStr"/>
-      <c r="AS3" t="inlineStr"/>
+      <c r="AS3" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
       <c r="AT3" t="inlineStr"/>
-      <c r="AU3" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="AV3" t="inlineStr"/>
+      <c r="AU3" t="inlineStr"/>
+      <c r="AV3" t="n">
+        <v>9.9</v>
+      </c>
       <c r="AW3" t="inlineStr"/>
       <c r="AX3" t="inlineStr"/>
       <c r="AY3" t="inlineStr"/>
-      <c r="AZ3" t="inlineStr"/>
-      <c r="BA3" t="inlineStr">
+      <c r="AZ3" t="inlineStr">
         <is>
           <t>praneeth</t>
         </is>
       </c>
+      <c r="BA3" t="inlineStr"/>
       <c r="BB3" t="inlineStr"/>
       <c r="BC3" t="inlineStr"/>
       <c r="BD3" t="inlineStr"/>
@@ -1640,15 +1650,17 @@
       <c r="BZ3" t="inlineStr"/>
       <c r="CA3" t="inlineStr"/>
       <c r="CB3" t="inlineStr"/>
-      <c r="CC3" t="inlineStr"/>
-      <c r="CD3" t="inlineStr">
+      <c r="CC3" t="inlineStr">
         <is>
           <t>Urban</t>
         </is>
       </c>
+      <c r="CD3" t="inlineStr"/>
       <c r="CE3" t="inlineStr"/>
       <c r="CF3" t="inlineStr"/>
-      <c r="CG3" t="inlineStr"/>
+      <c r="CG3" t="n">
+        <v>12.1</v>
+      </c>
       <c r="CH3" t="inlineStr"/>
       <c r="CI3" t="inlineStr"/>
       <c r="CJ3" t="inlineStr"/>
@@ -1789,142 +1801,140 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>14.8</v>
-      </c>
-      <c r="H4" t="n">
-        <v>16.4</v>
-      </c>
-      <c r="I4" t="n">
         <v>4.5</v>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>2026-02-23 05:27:05</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>60c2206a-8559-42c8-958b-171b5dfa66d5</t>
         </is>
       </c>
-      <c r="L4" t="n">
+      <c r="J4" t="n">
         <v>1</v>
       </c>
+      <c r="K4" t="n">
+        <v>3</v>
+      </c>
+      <c r="L4" t="inlineStr"/>
       <c r="M4" t="n">
-        <v>3</v>
-      </c>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="n">
         <v>1</v>
       </c>
-      <c r="P4" t="n">
+      <c r="N4" t="n">
         <v>1</v>
       </c>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr">
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr">
         <is>
           <t>SC</t>
         </is>
       </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Anaemic</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr">
         <is>
-          <t>Anaemic</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr">
-        <is>
           <t>0 – Calm and cooperative</t>
         </is>
       </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>Masimo Rad-67</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr"/>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>Masimo Rad-67</t>
-        </is>
-      </c>
-      <c r="AA4" t="inlineStr"/>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>Vegetarian</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr"/>
       <c r="AC4" t="inlineStr">
         <is>
-          <t>Vegetarian</t>
-        </is>
-      </c>
-      <c r="AD4" t="inlineStr"/>
-      <c r="AE4" t="inlineStr">
-        <is>
           <t>2024-07-24</t>
         </is>
       </c>
-      <c r="AF4" t="inlineStr">
+      <c r="AD4" t="inlineStr">
         <is>
           <t>Profession / Honours (Score 7)</t>
         </is>
       </c>
-      <c r="AG4" t="inlineStr"/>
-      <c r="AH4" t="inlineStr"/>
-      <c r="AI4" t="inlineStr">
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr">
         <is>
           <t>LECI0003</t>
         </is>
       </c>
-      <c r="AJ4" t="inlineStr">
+      <c r="AH4" t="inlineStr">
         <is>
           <t>2026-02-18 12:19:02</t>
         </is>
       </c>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr"/>
       <c r="AK4" t="inlineStr"/>
-      <c r="AL4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr">
+        <is>
+          <t>Nuclear</t>
+        </is>
+      </c>
       <c r="AM4" t="inlineStr"/>
-      <c r="AN4" t="inlineStr">
-        <is>
-          <t>Nuclear</t>
-        </is>
-      </c>
+      <c r="AN4" t="inlineStr"/>
       <c r="AO4" t="inlineStr"/>
       <c r="AP4" t="inlineStr"/>
       <c r="AQ4" t="inlineStr"/>
       <c r="AR4" t="inlineStr"/>
-      <c r="AS4" t="inlineStr"/>
+      <c r="AS4" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
       <c r="AT4" t="inlineStr"/>
-      <c r="AU4" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="AV4" t="inlineStr"/>
+      <c r="AU4" t="inlineStr"/>
+      <c r="AV4" t="n">
+        <v>16.4</v>
+      </c>
       <c r="AW4" t="inlineStr"/>
       <c r="AX4" t="inlineStr"/>
       <c r="AY4" t="inlineStr"/>
       <c r="AZ4" t="inlineStr"/>
       <c r="BA4" t="inlineStr"/>
       <c r="BB4" t="inlineStr"/>
-      <c r="BC4" t="inlineStr"/>
+      <c r="BC4" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
       <c r="BD4" t="inlineStr">
         <is>
-          <t>Daily</t>
-        </is>
-      </c>
-      <c r="BE4" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BE4" t="inlineStr"/>
       <c r="BF4" t="inlineStr"/>
       <c r="BG4" t="inlineStr"/>
       <c r="BH4" t="inlineStr"/>
@@ -1948,19 +1958,21 @@
       <c r="BZ4" t="inlineStr"/>
       <c r="CA4" t="inlineStr"/>
       <c r="CB4" t="inlineStr"/>
-      <c r="CC4" t="inlineStr"/>
-      <c r="CD4" t="inlineStr">
+      <c r="CC4" t="inlineStr">
         <is>
           <t>Urban</t>
         </is>
       </c>
-      <c r="CE4" t="inlineStr"/>
-      <c r="CF4" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="CG4" t="inlineStr"/>
+      <c r="CD4" t="inlineStr"/>
+      <c r="CE4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="CF4" t="inlineStr"/>
+      <c r="CG4" t="n">
+        <v>14.8</v>
+      </c>
       <c r="CH4" t="inlineStr"/>
       <c r="CI4" t="inlineStr"/>
       <c r="CJ4" t="inlineStr"/>
@@ -2115,19 +2127,15 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>14.5</v>
-      </c>
-      <c r="H5" t="n">
-        <v>14</v>
-      </c>
-      <c r="I5" t="n">
         <v>4.3</v>
       </c>
-      <c r="J5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="n">
+        <v>2</v>
+      </c>
       <c r="K5" t="inlineStr"/>
-      <c r="L5" t="n">
-        <v>2</v>
-      </c>
+      <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
@@ -2144,13 +2152,13 @@
       <c r="Z5" t="inlineStr"/>
       <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="inlineStr"/>
-      <c r="AC5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>2023-06-18</t>
+        </is>
+      </c>
       <c r="AD5" t="inlineStr"/>
-      <c r="AE5" t="inlineStr">
-        <is>
-          <t>2023-06-18</t>
-        </is>
-      </c>
+      <c r="AE5" t="inlineStr"/>
       <c r="AF5" t="inlineStr"/>
       <c r="AG5" t="inlineStr"/>
       <c r="AH5" t="inlineStr"/>
@@ -2164,14 +2172,16 @@
       <c r="AP5" t="inlineStr"/>
       <c r="AQ5" t="inlineStr"/>
       <c r="AR5" t="inlineStr"/>
-      <c r="AS5" t="inlineStr"/>
+      <c r="AS5" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
       <c r="AT5" t="inlineStr"/>
-      <c r="AU5" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="AV5" t="inlineStr"/>
+      <c r="AU5" t="inlineStr"/>
+      <c r="AV5" t="n">
+        <v>14</v>
+      </c>
       <c r="AW5" t="inlineStr"/>
       <c r="AX5" t="inlineStr"/>
       <c r="AY5" t="inlineStr"/>
@@ -2208,7 +2218,9 @@
       <c r="CD5" t="inlineStr"/>
       <c r="CE5" t="inlineStr"/>
       <c r="CF5" t="inlineStr"/>
-      <c r="CG5" t="inlineStr"/>
+      <c r="CG5" t="n">
+        <v>14.5</v>
+      </c>
       <c r="CH5" t="inlineStr"/>
       <c r="CI5" t="inlineStr"/>
       <c r="CJ5" t="inlineStr"/>
@@ -2322,18 +2334,14 @@
           <t>A</t>
         </is>
       </c>
-      <c r="G6" t="n">
-        <v>11.6</v>
-      </c>
-      <c r="H6" t="n">
-        <v>12</v>
-      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
+      <c r="J6" t="n">
+        <v>2</v>
+      </c>
       <c r="K6" t="inlineStr"/>
-      <c r="L6" t="n">
-        <v>2</v>
-      </c>
+      <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
@@ -2350,13 +2358,13 @@
       <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr"/>
-      <c r="AC6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>2023-06-18</t>
+        </is>
+      </c>
       <c r="AD6" t="inlineStr"/>
-      <c r="AE6" t="inlineStr">
-        <is>
-          <t>2023-06-18</t>
-        </is>
-      </c>
+      <c r="AE6" t="inlineStr"/>
       <c r="AF6" t="inlineStr"/>
       <c r="AG6" t="inlineStr"/>
       <c r="AH6" t="inlineStr"/>
@@ -2370,14 +2378,16 @@
       <c r="AP6" t="inlineStr"/>
       <c r="AQ6" t="inlineStr"/>
       <c r="AR6" t="inlineStr"/>
-      <c r="AS6" t="inlineStr"/>
+      <c r="AS6" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
       <c r="AT6" t="inlineStr"/>
-      <c r="AU6" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="AV6" t="inlineStr"/>
+      <c r="AU6" t="inlineStr"/>
+      <c r="AV6" t="n">
+        <v>12</v>
+      </c>
       <c r="AW6" t="inlineStr"/>
       <c r="AX6" t="inlineStr"/>
       <c r="AY6" t="inlineStr"/>
@@ -2414,7 +2424,9 @@
       <c r="CD6" t="inlineStr"/>
       <c r="CE6" t="inlineStr"/>
       <c r="CF6" t="inlineStr"/>
-      <c r="CG6" t="inlineStr"/>
+      <c r="CG6" t="n">
+        <v>11.6</v>
+      </c>
       <c r="CH6" t="inlineStr"/>
       <c r="CI6" t="inlineStr"/>
       <c r="CJ6" t="inlineStr"/>
@@ -2528,18 +2540,14 @@
           <t>F</t>
         </is>
       </c>
-      <c r="G7" t="n">
-        <v>11.9</v>
-      </c>
-      <c r="H7" t="n">
-        <v>13.1</v>
-      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="J7" t="n">
+        <v>2</v>
+      </c>
       <c r="K7" t="inlineStr"/>
-      <c r="L7" t="n">
-        <v>2</v>
-      </c>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
@@ -2556,13 +2564,13 @@
       <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr"/>
-      <c r="AC7" t="inlineStr"/>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>2023-06-15</t>
+        </is>
+      </c>
       <c r="AD7" t="inlineStr"/>
-      <c r="AE7" t="inlineStr">
-        <is>
-          <t>2023-06-15</t>
-        </is>
-      </c>
+      <c r="AE7" t="inlineStr"/>
       <c r="AF7" t="inlineStr"/>
       <c r="AG7" t="inlineStr"/>
       <c r="AH7" t="inlineStr"/>
@@ -2576,14 +2584,16 @@
       <c r="AP7" t="inlineStr"/>
       <c r="AQ7" t="inlineStr"/>
       <c r="AR7" t="inlineStr"/>
-      <c r="AS7" t="inlineStr"/>
+      <c r="AS7" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
       <c r="AT7" t="inlineStr"/>
-      <c r="AU7" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="AV7" t="inlineStr"/>
+      <c r="AU7" t="inlineStr"/>
+      <c r="AV7" t="n">
+        <v>13.1</v>
+      </c>
       <c r="AW7" t="inlineStr"/>
       <c r="AX7" t="inlineStr"/>
       <c r="AY7" t="inlineStr"/>
@@ -2620,7 +2630,9 @@
       <c r="CD7" t="inlineStr"/>
       <c r="CE7" t="inlineStr"/>
       <c r="CF7" t="inlineStr"/>
-      <c r="CG7" t="inlineStr"/>
+      <c r="CG7" t="n">
+        <v>11.9</v>
+      </c>
       <c r="CH7" t="inlineStr"/>
       <c r="CI7" t="inlineStr"/>
       <c r="CJ7" t="inlineStr"/>
@@ -2734,18 +2746,14 @@
           <t>A</t>
         </is>
       </c>
-      <c r="G8" t="n">
-        <v>11.5</v>
-      </c>
-      <c r="H8" t="n">
-        <v>10.8</v>
-      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
+      <c r="J8" t="n">
+        <v>2</v>
+      </c>
       <c r="K8" t="inlineStr"/>
-      <c r="L8" t="n">
-        <v>2</v>
-      </c>
+      <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
@@ -2762,13 +2770,13 @@
       <c r="Z8" t="inlineStr"/>
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr"/>
-      <c r="AC8" t="inlineStr"/>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>2023-03-08</t>
+        </is>
+      </c>
       <c r="AD8" t="inlineStr"/>
-      <c r="AE8" t="inlineStr">
-        <is>
-          <t>2023-03-08</t>
-        </is>
-      </c>
+      <c r="AE8" t="inlineStr"/>
       <c r="AF8" t="inlineStr"/>
       <c r="AG8" t="inlineStr"/>
       <c r="AH8" t="inlineStr"/>
@@ -2782,14 +2790,16 @@
       <c r="AP8" t="inlineStr"/>
       <c r="AQ8" t="inlineStr"/>
       <c r="AR8" t="inlineStr"/>
-      <c r="AS8" t="inlineStr"/>
+      <c r="AS8" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
       <c r="AT8" t="inlineStr"/>
-      <c r="AU8" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="AV8" t="inlineStr"/>
+      <c r="AU8" t="inlineStr"/>
+      <c r="AV8" t="n">
+        <v>10.8</v>
+      </c>
       <c r="AW8" t="inlineStr"/>
       <c r="AX8" t="inlineStr"/>
       <c r="AY8" t="inlineStr"/>
@@ -2826,7 +2836,9 @@
       <c r="CD8" t="inlineStr"/>
       <c r="CE8" t="inlineStr"/>
       <c r="CF8" t="inlineStr"/>
-      <c r="CG8" t="inlineStr"/>
+      <c r="CG8" t="n">
+        <v>11.5</v>
+      </c>
       <c r="CH8" t="inlineStr"/>
       <c r="CI8" t="inlineStr"/>
       <c r="CJ8" t="inlineStr"/>
@@ -2941,92 +2953,96 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>10.8</v>
-      </c>
-      <c r="H9" t="n">
-        <v>10.4</v>
-      </c>
-      <c r="I9" t="n">
         <v>9.5</v>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>2026-02-23 06:16:03</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>68803fb0-f4e8-4777-a702-a7997882b8a4</t>
         </is>
       </c>
-      <c r="L9" t="n">
+      <c r="J9" t="n">
         <v>22</v>
       </c>
-      <c r="M9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>1</v>
+      </c>
       <c r="N9" t="inlineStr"/>
-      <c r="O9" t="n">
-        <v>1</v>
-      </c>
+      <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr">
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
       <c r="Z9" t="inlineStr"/>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Mixed</t>
         </is>
       </c>
       <c r="AB9" t="inlineStr"/>
       <c r="AC9" t="inlineStr">
         <is>
-          <t>Mixed</t>
+          <t>2004-01-25</t>
         </is>
       </c>
       <c r="AD9" t="inlineStr"/>
-      <c r="AE9" t="inlineStr">
-        <is>
-          <t>2004-01-25</t>
-        </is>
-      </c>
+      <c r="AE9" t="inlineStr"/>
       <c r="AF9" t="inlineStr"/>
       <c r="AG9" t="inlineStr"/>
       <c r="AH9" t="inlineStr"/>
       <c r="AI9" t="inlineStr"/>
-      <c r="AJ9" t="inlineStr"/>
+      <c r="AJ9" t="n">
+        <v>4</v>
+      </c>
       <c r="AK9" t="inlineStr"/>
-      <c r="AL9" t="n">
-        <v>4</v>
-      </c>
-      <c r="AM9" t="inlineStr"/>
+      <c r="AL9" t="inlineStr">
+        <is>
+          <t>Nuclear</t>
+        </is>
+      </c>
+      <c r="AM9" t="inlineStr">
+        <is>
+          <t>Rarely</t>
+        </is>
+      </c>
       <c r="AN9" t="inlineStr">
         <is>
-          <t>Nuclear</t>
+          <t>Daily</t>
         </is>
       </c>
       <c r="AO9" t="inlineStr">
         <is>
-          <t>Rarely</t>
+          <t>Daily</t>
         </is>
       </c>
       <c r="AP9" t="inlineStr">
         <is>
-          <t>Daily</t>
+          <t>3–4/week</t>
         </is>
       </c>
       <c r="AQ9" t="inlineStr">
         <is>
-          <t>Daily</t>
+          <t>1–2/week</t>
         </is>
       </c>
       <c r="AR9" t="inlineStr">
@@ -3036,58 +3052,54 @@
       </c>
       <c r="AS9" t="inlineStr">
         <is>
-          <t>1–2/week</t>
-        </is>
-      </c>
-      <c r="AT9" t="inlineStr">
-        <is>
-          <t>3–4/week</t>
-        </is>
-      </c>
-      <c r="AU9" t="inlineStr">
-        <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="AV9" t="inlineStr"/>
-      <c r="AW9" t="n">
+      <c r="AT9" t="inlineStr"/>
+      <c r="AU9" t="n">
         <v>156</v>
       </c>
+      <c r="AV9" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="AW9" t="inlineStr"/>
       <c r="AX9" t="inlineStr"/>
       <c r="AY9" t="inlineStr"/>
-      <c r="AZ9" t="inlineStr"/>
-      <c r="BA9" t="inlineStr">
+      <c r="AZ9" t="inlineStr">
         <is>
           <t>lekha</t>
         </is>
       </c>
+      <c r="BA9" t="inlineStr"/>
       <c r="BB9" t="inlineStr"/>
       <c r="BC9" t="inlineStr"/>
       <c r="BD9" t="inlineStr"/>
-      <c r="BE9" t="inlineStr"/>
-      <c r="BF9" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="BG9" t="n">
+      <c r="BE9" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BF9" t="n">
         <v>27</v>
       </c>
-      <c r="BH9" t="inlineStr"/>
-      <c r="BI9" t="n">
+      <c r="BG9" t="inlineStr"/>
+      <c r="BH9" t="n">
         <v>1</v>
       </c>
+      <c r="BI9" t="inlineStr">
+        <is>
+          <t>Easy</t>
+        </is>
+      </c>
       <c r="BJ9" t="inlineStr">
         <is>
-          <t>Easy</t>
-        </is>
-      </c>
-      <c r="BK9" t="inlineStr">
-        <is>
           <t>Very easy</t>
         </is>
       </c>
-      <c r="BL9" t="inlineStr"/>
+      <c r="BK9" t="inlineStr"/>
+      <c r="BL9" t="n">
+        <v>0</v>
+      </c>
       <c r="BM9" t="n">
         <v>0</v>
       </c>
@@ -3100,19 +3112,21 @@
       <c r="BP9" t="n">
         <v>0</v>
       </c>
-      <c r="BQ9" t="n">
-        <v>0</v>
-      </c>
+      <c r="BQ9" t="inlineStr"/>
       <c r="BR9" t="inlineStr"/>
-      <c r="BS9" t="inlineStr"/>
+      <c r="BS9" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
       <c r="BT9" t="inlineStr">
         <is>
-          <t>Daily</t>
+          <t>Highly portable</t>
         </is>
       </c>
       <c r="BU9" t="inlineStr">
         <is>
-          <t>Highly portable</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BV9" t="inlineStr">
@@ -3122,38 +3136,36 @@
       </c>
       <c r="BW9" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>Always</t>
         </is>
       </c>
       <c r="BX9" t="inlineStr">
         <is>
-          <t>Always</t>
-        </is>
-      </c>
-      <c r="BY9" t="inlineStr">
-        <is>
           <t>Very safe</t>
         </is>
       </c>
-      <c r="BZ9" t="inlineStr"/>
-      <c r="CA9" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="BY9" t="inlineStr"/>
+      <c r="BZ9" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="CA9" t="inlineStr"/>
       <c r="CB9" t="inlineStr"/>
       <c r="CC9" t="inlineStr"/>
-      <c r="CD9" t="inlineStr"/>
-      <c r="CE9" t="inlineStr">
+      <c r="CD9" t="inlineStr">
         <is>
           <t>Urban</t>
         </is>
       </c>
-      <c r="CF9" t="inlineStr"/>
-      <c r="CG9" t="inlineStr">
+      <c r="CE9" t="inlineStr"/>
+      <c r="CF9" t="inlineStr">
         <is>
           <t>No</t>
         </is>
+      </c>
+      <c r="CG9" t="n">
+        <v>10.8</v>
       </c>
       <c r="CH9" t="inlineStr"/>
       <c r="CI9" t="inlineStr">
@@ -4233,77 +4245,85 @@
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>2026-02-24 10:57:10</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>721c38a1-f418-46b5-9776-0077d9fcb40d</t>
         </is>
       </c>
-      <c r="L14" t="n">
+      <c r="J14" t="n">
         <v>5</v>
       </c>
-      <c r="M14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="n">
+        <v>1</v>
+      </c>
       <c r="N14" t="inlineStr"/>
-      <c r="O14" t="n">
-        <v>1</v>
-      </c>
+      <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Anaemic</t>
+        </is>
+      </c>
       <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>Anaemic</t>
-        </is>
-      </c>
+      <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="W14" t="inlineStr"/>
       <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="Z14" t="inlineStr"/>
       <c r="AA14" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>Vegetarian</t>
         </is>
       </c>
       <c r="AB14" t="inlineStr"/>
       <c r="AC14" t="inlineStr">
         <is>
-          <t>Vegetarian</t>
+          <t>2020-07-24</t>
         </is>
       </c>
       <c r="AD14" t="inlineStr"/>
-      <c r="AE14" t="inlineStr">
-        <is>
-          <t>2020-07-24</t>
-        </is>
+      <c r="AE14" t="n">
+        <v>7</v>
       </c>
       <c r="AF14" t="inlineStr"/>
-      <c r="AG14" t="n">
-        <v>7</v>
-      </c>
+      <c r="AG14" t="inlineStr"/>
       <c r="AH14" t="inlineStr"/>
-      <c r="AI14" t="inlineStr"/>
+      <c r="AI14" t="n">
+        <v>12</v>
+      </c>
       <c r="AJ14" t="inlineStr"/>
-      <c r="AK14" t="n">
-        <v>12</v>
-      </c>
-      <c r="AL14" t="inlineStr"/>
-      <c r="AM14" t="inlineStr"/>
+      <c r="AK14" t="inlineStr"/>
+      <c r="AL14" t="inlineStr">
+        <is>
+          <t>Nuclear</t>
+        </is>
+      </c>
+      <c r="AM14" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
       <c r="AN14" t="inlineStr">
         <is>
-          <t>Nuclear</t>
+          <t>Daily</t>
         </is>
       </c>
       <c r="AO14" t="inlineStr">
@@ -4326,16 +4346,8 @@
           <t>Daily</t>
         </is>
       </c>
-      <c r="AS14" t="inlineStr">
-        <is>
-          <t>Daily</t>
-        </is>
-      </c>
-      <c r="AT14" t="inlineStr">
-        <is>
-          <t>Daily</t>
-        </is>
-      </c>
+      <c r="AS14" t="inlineStr"/>
+      <c r="AT14" t="inlineStr"/>
       <c r="AU14" t="inlineStr"/>
       <c r="AV14" t="inlineStr"/>
       <c r="AW14" t="inlineStr"/>
@@ -4346,57 +4358,61 @@
       <c r="BB14" t="inlineStr"/>
       <c r="BC14" t="inlineStr"/>
       <c r="BD14" t="inlineStr"/>
-      <c r="BE14" t="inlineStr"/>
-      <c r="BF14" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="BG14" t="n">
+      <c r="BE14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BF14" t="n">
         <v>25</v>
       </c>
-      <c r="BH14" t="inlineStr"/>
-      <c r="BI14" t="n">
+      <c r="BG14" t="inlineStr"/>
+      <c r="BH14" t="n">
         <v>1</v>
       </c>
+      <c r="BI14" t="inlineStr">
+        <is>
+          <t>Easy</t>
+        </is>
+      </c>
       <c r="BJ14" t="inlineStr">
         <is>
-          <t>Easy</t>
-        </is>
-      </c>
-      <c r="BK14" t="inlineStr">
-        <is>
           <t>Very easy</t>
         </is>
       </c>
-      <c r="BL14" t="inlineStr"/>
+      <c r="BK14" t="inlineStr"/>
+      <c r="BL14" t="n">
+        <v>0</v>
+      </c>
       <c r="BM14" t="n">
         <v>0</v>
       </c>
       <c r="BN14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BO14" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP14" t="n">
         <v>2</v>
       </c>
-      <c r="BP14" t="n">
-        <v>0</v>
-      </c>
       <c r="BQ14" t="n">
-        <v>2</v>
-      </c>
-      <c r="BR14" t="n">
         <v>4</v>
       </c>
-      <c r="BS14" t="inlineStr"/>
+      <c r="BR14" t="inlineStr"/>
+      <c r="BS14" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
       <c r="BT14" t="inlineStr">
         <is>
-          <t>Daily</t>
+          <t>Highly portable</t>
         </is>
       </c>
       <c r="BU14" t="inlineStr">
         <is>
-          <t>Highly portable</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BV14" t="inlineStr">
@@ -4406,39 +4422,35 @@
       </c>
       <c r="BW14" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>Always</t>
         </is>
       </c>
       <c r="BX14" t="inlineStr">
         <is>
-          <t>Always</t>
-        </is>
-      </c>
-      <c r="BY14" t="inlineStr">
-        <is>
           <t>Very safe</t>
         </is>
       </c>
-      <c r="BZ14" t="inlineStr"/>
-      <c r="CA14" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="BY14" t="inlineStr"/>
+      <c r="BZ14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="CA14" t="inlineStr"/>
       <c r="CB14" t="inlineStr"/>
       <c r="CC14" t="inlineStr"/>
-      <c r="CD14" t="inlineStr"/>
-      <c r="CE14" t="inlineStr">
+      <c r="CD14" t="inlineStr">
         <is>
           <t>Urban</t>
         </is>
       </c>
-      <c r="CF14" t="inlineStr"/>
-      <c r="CG14" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="CE14" t="inlineStr"/>
+      <c r="CF14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="CG14" t="inlineStr"/>
       <c r="CH14" t="inlineStr"/>
       <c r="CI14" t="inlineStr">
         <is>
@@ -4729,77 +4741,85 @@
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>2026-02-24 11:08:04</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>cceb8dc2-a370-4dcc-b23b-568b05505c6d</t>
         </is>
       </c>
-      <c r="L15" t="n">
+      <c r="J15" t="n">
         <v>4</v>
       </c>
-      <c r="M15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="n">
+        <v>1</v>
+      </c>
       <c r="N15" t="inlineStr"/>
-      <c r="O15" t="n">
-        <v>1</v>
-      </c>
+      <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>Anaemic</t>
+        </is>
+      </c>
       <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>Anaemic</t>
-        </is>
-      </c>
+      <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
-      <c r="U15" t="inlineStr"/>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="V15" t="inlineStr"/>
-      <c r="W15" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="W15" t="inlineStr"/>
       <c r="X15" t="inlineStr"/>
-      <c r="Y15" t="inlineStr"/>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="Z15" t="inlineStr"/>
       <c r="AA15" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>Vegetarian</t>
         </is>
       </c>
       <c r="AB15" t="inlineStr"/>
       <c r="AC15" t="inlineStr">
         <is>
-          <t>Vegetarian</t>
+          <t>2021-06-16</t>
         </is>
       </c>
       <c r="AD15" t="inlineStr"/>
-      <c r="AE15" t="inlineStr">
-        <is>
-          <t>2021-06-16</t>
-        </is>
+      <c r="AE15" t="n">
+        <v>7</v>
       </c>
       <c r="AF15" t="inlineStr"/>
-      <c r="AG15" t="n">
-        <v>7</v>
-      </c>
+      <c r="AG15" t="inlineStr"/>
       <c r="AH15" t="inlineStr"/>
-      <c r="AI15" t="inlineStr"/>
+      <c r="AI15" t="n">
+        <v>12</v>
+      </c>
       <c r="AJ15" t="inlineStr"/>
-      <c r="AK15" t="n">
-        <v>12</v>
-      </c>
-      <c r="AL15" t="inlineStr"/>
-      <c r="AM15" t="inlineStr"/>
+      <c r="AK15" t="inlineStr"/>
+      <c r="AL15" t="inlineStr">
+        <is>
+          <t>Nuclear</t>
+        </is>
+      </c>
+      <c r="AM15" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
       <c r="AN15" t="inlineStr">
         <is>
-          <t>Nuclear</t>
+          <t>Daily</t>
         </is>
       </c>
       <c r="AO15" t="inlineStr">
@@ -4822,16 +4842,8 @@
           <t>Daily</t>
         </is>
       </c>
-      <c r="AS15" t="inlineStr">
-        <is>
-          <t>Daily</t>
-        </is>
-      </c>
-      <c r="AT15" t="inlineStr">
-        <is>
-          <t>Daily</t>
-        </is>
-      </c>
+      <c r="AS15" t="inlineStr"/>
+      <c r="AT15" t="inlineStr"/>
       <c r="AU15" t="inlineStr"/>
       <c r="AV15" t="inlineStr"/>
       <c r="AW15" t="inlineStr"/>
@@ -4842,28 +4854,30 @@
       <c r="BB15" t="inlineStr"/>
       <c r="BC15" t="inlineStr"/>
       <c r="BD15" t="inlineStr"/>
-      <c r="BE15" t="inlineStr"/>
-      <c r="BF15" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="BE15" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BF15" t="inlineStr"/>
       <c r="BG15" t="inlineStr"/>
-      <c r="BH15" t="inlineStr"/>
-      <c r="BI15" t="n">
+      <c r="BH15" t="n">
         <v>1</v>
       </c>
+      <c r="BI15" t="inlineStr">
+        <is>
+          <t>Easy</t>
+        </is>
+      </c>
       <c r="BJ15" t="inlineStr">
         <is>
-          <t>Easy</t>
-        </is>
-      </c>
-      <c r="BK15" t="inlineStr">
-        <is>
           <t>Very easy</t>
         </is>
       </c>
-      <c r="BL15" t="inlineStr"/>
+      <c r="BK15" t="inlineStr"/>
+      <c r="BL15" t="n">
+        <v>0</v>
+      </c>
       <c r="BM15" t="n">
         <v>0</v>
       </c>
@@ -4879,18 +4893,20 @@
       <c r="BQ15" t="n">
         <v>0</v>
       </c>
-      <c r="BR15" t="n">
-        <v>0</v>
-      </c>
-      <c r="BS15" t="inlineStr"/>
+      <c r="BR15" t="inlineStr"/>
+      <c r="BS15" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
       <c r="BT15" t="inlineStr">
         <is>
-          <t>Daily</t>
+          <t>Highly portable</t>
         </is>
       </c>
       <c r="BU15" t="inlineStr">
         <is>
-          <t>Highly portable</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BV15" t="inlineStr">
@@ -4900,39 +4916,35 @@
       </c>
       <c r="BW15" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>Always</t>
         </is>
       </c>
       <c r="BX15" t="inlineStr">
         <is>
-          <t>Always</t>
-        </is>
-      </c>
-      <c r="BY15" t="inlineStr">
-        <is>
           <t>Very safe</t>
         </is>
       </c>
-      <c r="BZ15" t="inlineStr"/>
-      <c r="CA15" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="BY15" t="inlineStr"/>
+      <c r="BZ15" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="CA15" t="inlineStr"/>
       <c r="CB15" t="inlineStr"/>
       <c r="CC15" t="inlineStr"/>
-      <c r="CD15" t="inlineStr"/>
-      <c r="CE15" t="inlineStr">
+      <c r="CD15" t="inlineStr">
         <is>
           <t>Urban</t>
         </is>
       </c>
-      <c r="CF15" t="inlineStr"/>
-      <c r="CG15" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="CE15" t="inlineStr"/>
+      <c r="CF15" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="CG15" t="inlineStr"/>
       <c r="CH15" t="inlineStr"/>
       <c r="CI15" t="inlineStr">
         <is>
@@ -6589,77 +6601,85 @@
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr">
+      <c r="H23" t="inlineStr">
         <is>
           <t>2026-02-26 12:45:03</t>
         </is>
       </c>
-      <c r="K23" t="inlineStr">
+      <c r="I23" t="inlineStr">
         <is>
           <t>54f1adf7-5aad-4204-b55e-9c4f40fd0252</t>
         </is>
       </c>
-      <c r="L23" t="n">
+      <c r="J23" t="n">
         <v>3</v>
       </c>
-      <c r="M23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="n">
+        <v>1</v>
+      </c>
       <c r="N23" t="inlineStr"/>
-      <c r="O23" t="n">
-        <v>1</v>
-      </c>
+      <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>Anaemic</t>
+        </is>
+      </c>
       <c r="R23" t="inlineStr"/>
-      <c r="S23" t="inlineStr">
-        <is>
-          <t>Anaemic</t>
-        </is>
-      </c>
+      <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
-      <c r="U23" t="inlineStr"/>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="V23" t="inlineStr"/>
-      <c r="W23" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="W23" t="inlineStr"/>
       <c r="X23" t="inlineStr"/>
-      <c r="Y23" t="inlineStr"/>
+      <c r="Y23" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="Z23" t="inlineStr"/>
       <c r="AA23" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>Vegetarian</t>
         </is>
       </c>
       <c r="AB23" t="inlineStr"/>
       <c r="AC23" t="inlineStr">
         <is>
-          <t>Vegetarian</t>
+          <t>2022-07-15</t>
         </is>
       </c>
       <c r="AD23" t="inlineStr"/>
-      <c r="AE23" t="inlineStr">
-        <is>
-          <t>2022-07-15</t>
-        </is>
+      <c r="AE23" t="n">
+        <v>7</v>
       </c>
       <c r="AF23" t="inlineStr"/>
-      <c r="AG23" t="n">
-        <v>7</v>
-      </c>
+      <c r="AG23" t="inlineStr"/>
       <c r="AH23" t="inlineStr"/>
-      <c r="AI23" t="inlineStr"/>
+      <c r="AI23" t="n">
+        <v>12</v>
+      </c>
       <c r="AJ23" t="inlineStr"/>
-      <c r="AK23" t="n">
-        <v>12</v>
-      </c>
-      <c r="AL23" t="inlineStr"/>
-      <c r="AM23" t="inlineStr"/>
+      <c r="AK23" t="inlineStr"/>
+      <c r="AL23" t="inlineStr">
+        <is>
+          <t>Nuclear</t>
+        </is>
+      </c>
+      <c r="AM23" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
       <c r="AN23" t="inlineStr">
         <is>
-          <t>Nuclear</t>
+          <t>Daily</t>
         </is>
       </c>
       <c r="AO23" t="inlineStr">
@@ -6682,52 +6702,46 @@
           <t>Daily</t>
         </is>
       </c>
-      <c r="AS23" t="inlineStr">
-        <is>
-          <t>Daily</t>
-        </is>
-      </c>
-      <c r="AT23" t="inlineStr">
-        <is>
-          <t>Daily</t>
-        </is>
-      </c>
+      <c r="AS23" t="inlineStr"/>
+      <c r="AT23" t="inlineStr"/>
       <c r="AU23" t="inlineStr"/>
       <c r="AV23" t="inlineStr"/>
-      <c r="AW23" t="inlineStr"/>
-      <c r="AX23" t="inlineStr">
+      <c r="AW23" t="inlineStr">
         <is>
           <t>13+4</t>
         </is>
       </c>
+      <c r="AX23" t="inlineStr"/>
       <c r="AY23" t="inlineStr"/>
       <c r="AZ23" t="inlineStr"/>
       <c r="BA23" t="inlineStr"/>
       <c r="BB23" t="inlineStr"/>
       <c r="BC23" t="inlineStr"/>
       <c r="BD23" t="inlineStr"/>
-      <c r="BE23" t="inlineStr"/>
-      <c r="BF23" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="BE23" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BF23" t="inlineStr"/>
       <c r="BG23" t="inlineStr"/>
-      <c r="BH23" t="inlineStr"/>
-      <c r="BI23" t="n">
+      <c r="BH23" t="n">
         <v>1</v>
       </c>
+      <c r="BI23" t="inlineStr">
+        <is>
+          <t>Easy</t>
+        </is>
+      </c>
       <c r="BJ23" t="inlineStr">
         <is>
-          <t>Easy</t>
-        </is>
-      </c>
-      <c r="BK23" t="inlineStr">
-        <is>
           <t>Very easy</t>
         </is>
       </c>
-      <c r="BL23" t="inlineStr"/>
+      <c r="BK23" t="inlineStr"/>
+      <c r="BL23" t="n">
+        <v>0</v>
+      </c>
       <c r="BM23" t="n">
         <v>0</v>
       </c>
@@ -6743,18 +6757,20 @@
       <c r="BQ23" t="n">
         <v>0</v>
       </c>
-      <c r="BR23" t="n">
-        <v>0</v>
-      </c>
-      <c r="BS23" t="inlineStr"/>
+      <c r="BR23" t="inlineStr"/>
+      <c r="BS23" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
       <c r="BT23" t="inlineStr">
         <is>
-          <t>Daily</t>
+          <t>Highly portable</t>
         </is>
       </c>
       <c r="BU23" t="inlineStr">
         <is>
-          <t>Highly portable</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BV23" t="inlineStr">
@@ -6764,39 +6780,35 @@
       </c>
       <c r="BW23" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>Always</t>
         </is>
       </c>
       <c r="BX23" t="inlineStr">
         <is>
-          <t>Always</t>
-        </is>
-      </c>
-      <c r="BY23" t="inlineStr">
-        <is>
           <t>Very safe</t>
         </is>
       </c>
-      <c r="BZ23" t="inlineStr"/>
-      <c r="CA23" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="BY23" t="inlineStr"/>
+      <c r="BZ23" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="CA23" t="inlineStr"/>
       <c r="CB23" t="inlineStr"/>
       <c r="CC23" t="inlineStr"/>
-      <c r="CD23" t="inlineStr"/>
-      <c r="CE23" t="inlineStr">
+      <c r="CD23" t="inlineStr">
         <is>
           <t>Urban</t>
         </is>
       </c>
-      <c r="CF23" t="inlineStr"/>
-      <c r="CG23" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="CE23" t="inlineStr"/>
+      <c r="CF23" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="CG23" t="inlineStr"/>
       <c r="CH23" t="inlineStr"/>
       <c r="CI23" t="inlineStr">
         <is>
@@ -7669,77 +7681,85 @@
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr">
+      <c r="H27" t="inlineStr">
         <is>
           <t>2026-02-26 16:42:45</t>
         </is>
       </c>
-      <c r="K27" t="inlineStr">
+      <c r="I27" t="inlineStr">
         <is>
           <t>099b6f0e-b26e-4389-8f4d-1b931a61f88b</t>
         </is>
       </c>
-      <c r="L27" t="n">
+      <c r="J27" t="n">
         <v>3</v>
       </c>
-      <c r="M27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="n">
+        <v>1</v>
+      </c>
       <c r="N27" t="inlineStr"/>
-      <c r="O27" t="n">
-        <v>1</v>
-      </c>
+      <c r="O27" t="inlineStr"/>
       <c r="P27" t="inlineStr"/>
-      <c r="Q27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>Anaemic</t>
+        </is>
+      </c>
       <c r="R27" t="inlineStr"/>
-      <c r="S27" t="inlineStr">
-        <is>
-          <t>Anaemic</t>
-        </is>
-      </c>
+      <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr"/>
-      <c r="U27" t="inlineStr"/>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="V27" t="inlineStr"/>
-      <c r="W27" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="W27" t="inlineStr"/>
       <c r="X27" t="inlineStr"/>
-      <c r="Y27" t="inlineStr"/>
+      <c r="Y27" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="Z27" t="inlineStr"/>
       <c r="AA27" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>Vegetarian</t>
         </is>
       </c>
       <c r="AB27" t="inlineStr"/>
       <c r="AC27" t="inlineStr">
         <is>
-          <t>Vegetarian</t>
+          <t>2022-11-19</t>
         </is>
       </c>
       <c r="AD27" t="inlineStr"/>
-      <c r="AE27" t="inlineStr">
-        <is>
-          <t>2022-11-19</t>
-        </is>
+      <c r="AE27" t="n">
+        <v>7</v>
       </c>
       <c r="AF27" t="inlineStr"/>
-      <c r="AG27" t="n">
-        <v>7</v>
-      </c>
+      <c r="AG27" t="inlineStr"/>
       <c r="AH27" t="inlineStr"/>
-      <c r="AI27" t="inlineStr"/>
+      <c r="AI27" t="n">
+        <v>12</v>
+      </c>
       <c r="AJ27" t="inlineStr"/>
-      <c r="AK27" t="n">
-        <v>12</v>
-      </c>
-      <c r="AL27" t="inlineStr"/>
-      <c r="AM27" t="inlineStr"/>
+      <c r="AK27" t="inlineStr"/>
+      <c r="AL27" t="inlineStr">
+        <is>
+          <t>Nuclear</t>
+        </is>
+      </c>
+      <c r="AM27" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
       <c r="AN27" t="inlineStr">
         <is>
-          <t>Nuclear</t>
+          <t>Daily</t>
         </is>
       </c>
       <c r="AO27" t="inlineStr">
@@ -7762,60 +7782,54 @@
           <t>Daily</t>
         </is>
       </c>
-      <c r="AS27" t="inlineStr">
-        <is>
-          <t>Daily</t>
-        </is>
-      </c>
-      <c r="AT27" t="inlineStr">
-        <is>
-          <t>Daily</t>
-        </is>
-      </c>
+      <c r="AS27" t="inlineStr"/>
+      <c r="AT27" t="inlineStr"/>
       <c r="AU27" t="inlineStr"/>
       <c r="AV27" t="inlineStr"/>
-      <c r="AW27" t="inlineStr"/>
-      <c r="AX27" t="inlineStr">
+      <c r="AW27" t="inlineStr">
         <is>
           <t>Enter valid Weight + Horiba Hb</t>
         </is>
       </c>
+      <c r="AX27" t="inlineStr"/>
       <c r="AY27" t="inlineStr"/>
-      <c r="AZ27" t="inlineStr"/>
-      <c r="BA27" t="inlineStr">
+      <c r="AZ27" t="inlineStr">
         <is>
           <t>Jahnavi</t>
         </is>
       </c>
-      <c r="BB27" t="inlineStr"/>
-      <c r="BC27" t="inlineStr">
+      <c r="BA27" t="inlineStr"/>
+      <c r="BB27" t="inlineStr">
         <is>
           <t>Jahnavi</t>
         </is>
       </c>
+      <c r="BC27" t="inlineStr"/>
       <c r="BD27" t="inlineStr"/>
-      <c r="BE27" t="inlineStr"/>
-      <c r="BF27" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="BE27" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BF27" t="inlineStr"/>
       <c r="BG27" t="inlineStr"/>
-      <c r="BH27" t="inlineStr"/>
-      <c r="BI27" t="n">
+      <c r="BH27" t="n">
         <v>1</v>
       </c>
+      <c r="BI27" t="inlineStr">
+        <is>
+          <t>Easy</t>
+        </is>
+      </c>
       <c r="BJ27" t="inlineStr">
         <is>
-          <t>Easy</t>
-        </is>
-      </c>
-      <c r="BK27" t="inlineStr">
-        <is>
           <t>Very easy</t>
         </is>
       </c>
-      <c r="BL27" t="inlineStr"/>
+      <c r="BK27" t="inlineStr"/>
+      <c r="BL27" t="n">
+        <v>0</v>
+      </c>
       <c r="BM27" t="n">
         <v>0</v>
       </c>
@@ -7831,18 +7845,20 @@
       <c r="BQ27" t="n">
         <v>0</v>
       </c>
-      <c r="BR27" t="n">
-        <v>0</v>
-      </c>
-      <c r="BS27" t="inlineStr"/>
+      <c r="BR27" t="inlineStr"/>
+      <c r="BS27" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
       <c r="BT27" t="inlineStr">
         <is>
-          <t>Daily</t>
+          <t>Highly portable</t>
         </is>
       </c>
       <c r="BU27" t="inlineStr">
         <is>
-          <t>Highly portable</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BV27" t="inlineStr">
@@ -7852,39 +7868,35 @@
       </c>
       <c r="BW27" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>Always</t>
         </is>
       </c>
       <c r="BX27" t="inlineStr">
         <is>
-          <t>Always</t>
-        </is>
-      </c>
-      <c r="BY27" t="inlineStr">
-        <is>
           <t>Very safe</t>
         </is>
       </c>
-      <c r="BZ27" t="inlineStr"/>
-      <c r="CA27" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="BY27" t="inlineStr"/>
+      <c r="BZ27" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="CA27" t="inlineStr"/>
       <c r="CB27" t="inlineStr"/>
       <c r="CC27" t="inlineStr"/>
-      <c r="CD27" t="inlineStr"/>
-      <c r="CE27" t="inlineStr">
+      <c r="CD27" t="inlineStr">
         <is>
           <t>Urban</t>
         </is>
       </c>
-      <c r="CF27" t="inlineStr"/>
-      <c r="CG27" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="CE27" t="inlineStr"/>
+      <c r="CF27" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="CG27" t="inlineStr"/>
       <c r="CH27" t="inlineStr"/>
       <c r="CI27" t="inlineStr">
         <is>
@@ -8169,77 +8181,85 @@
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr">
+      <c r="H28" t="inlineStr">
         <is>
           <t>2026-02-26 18:01:27</t>
         </is>
       </c>
-      <c r="K28" t="inlineStr">
+      <c r="I28" t="inlineStr">
         <is>
           <t>8a35e6f4-38fe-41e5-8d3e-d7ca8557f7a2</t>
         </is>
       </c>
-      <c r="L28" t="n">
+      <c r="J28" t="n">
         <v>3</v>
       </c>
-      <c r="M28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="n">
+        <v>1</v>
+      </c>
       <c r="N28" t="inlineStr"/>
-      <c r="O28" t="n">
-        <v>1</v>
-      </c>
+      <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr"/>
-      <c r="Q28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>Anaemic</t>
+        </is>
+      </c>
       <c r="R28" t="inlineStr"/>
-      <c r="S28" t="inlineStr">
-        <is>
-          <t>Anaemic</t>
-        </is>
-      </c>
+      <c r="S28" t="inlineStr"/>
       <c r="T28" t="inlineStr"/>
-      <c r="U28" t="inlineStr"/>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="V28" t="inlineStr"/>
-      <c r="W28" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="W28" t="inlineStr"/>
       <c r="X28" t="inlineStr"/>
-      <c r="Y28" t="inlineStr"/>
+      <c r="Y28" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="Z28" t="inlineStr"/>
       <c r="AA28" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>Vegetarian</t>
         </is>
       </c>
       <c r="AB28" t="inlineStr"/>
       <c r="AC28" t="inlineStr">
         <is>
-          <t>Vegetarian</t>
+          <t>2022-11-18</t>
         </is>
       </c>
       <c r="AD28" t="inlineStr"/>
-      <c r="AE28" t="inlineStr">
-        <is>
-          <t>2022-11-18</t>
-        </is>
+      <c r="AE28" t="n">
+        <v>7</v>
       </c>
       <c r="AF28" t="inlineStr"/>
-      <c r="AG28" t="n">
-        <v>7</v>
-      </c>
+      <c r="AG28" t="inlineStr"/>
       <c r="AH28" t="inlineStr"/>
-      <c r="AI28" t="inlineStr"/>
+      <c r="AI28" t="n">
+        <v>12</v>
+      </c>
       <c r="AJ28" t="inlineStr"/>
-      <c r="AK28" t="n">
-        <v>12</v>
-      </c>
-      <c r="AL28" t="inlineStr"/>
-      <c r="AM28" t="inlineStr"/>
+      <c r="AK28" t="inlineStr"/>
+      <c r="AL28" t="inlineStr">
+        <is>
+          <t>Nuclear</t>
+        </is>
+      </c>
+      <c r="AM28" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
       <c r="AN28" t="inlineStr">
         <is>
-          <t>Nuclear</t>
+          <t>Daily</t>
         </is>
       </c>
       <c r="AO28" t="inlineStr">
@@ -8262,60 +8282,54 @@
           <t>Daily</t>
         </is>
       </c>
-      <c r="AS28" t="inlineStr">
-        <is>
-          <t>Daily</t>
-        </is>
-      </c>
-      <c r="AT28" t="inlineStr">
-        <is>
-          <t>Daily</t>
-        </is>
-      </c>
+      <c r="AS28" t="inlineStr"/>
+      <c r="AT28" t="inlineStr"/>
       <c r="AU28" t="inlineStr"/>
       <c r="AV28" t="inlineStr"/>
-      <c r="AW28" t="inlineStr"/>
-      <c r="AX28" t="inlineStr">
+      <c r="AW28" t="inlineStr">
         <is>
           <t>Enter valid Weight + Horiba Hb</t>
         </is>
       </c>
+      <c r="AX28" t="inlineStr"/>
       <c r="AY28" t="inlineStr"/>
-      <c r="AZ28" t="inlineStr"/>
-      <c r="BA28" t="inlineStr">
+      <c r="AZ28" t="inlineStr">
         <is>
           <t>Jahnavi</t>
         </is>
       </c>
-      <c r="BB28" t="inlineStr"/>
-      <c r="BC28" t="inlineStr">
+      <c r="BA28" t="inlineStr"/>
+      <c r="BB28" t="inlineStr">
         <is>
           <t>Jahnavi</t>
         </is>
       </c>
+      <c r="BC28" t="inlineStr"/>
       <c r="BD28" t="inlineStr"/>
-      <c r="BE28" t="inlineStr"/>
-      <c r="BF28" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="BE28" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BF28" t="inlineStr"/>
       <c r="BG28" t="inlineStr"/>
-      <c r="BH28" t="inlineStr"/>
-      <c r="BI28" t="n">
+      <c r="BH28" t="n">
         <v>1</v>
       </c>
+      <c r="BI28" t="inlineStr">
+        <is>
+          <t>Easy</t>
+        </is>
+      </c>
       <c r="BJ28" t="inlineStr">
         <is>
-          <t>Easy</t>
-        </is>
-      </c>
-      <c r="BK28" t="inlineStr">
-        <is>
           <t>Very easy</t>
         </is>
       </c>
-      <c r="BL28" t="inlineStr"/>
+      <c r="BK28" t="inlineStr"/>
+      <c r="BL28" t="n">
+        <v>0</v>
+      </c>
       <c r="BM28" t="n">
         <v>0</v>
       </c>
@@ -8331,18 +8345,20 @@
       <c r="BQ28" t="n">
         <v>0</v>
       </c>
-      <c r="BR28" t="n">
-        <v>0</v>
-      </c>
-      <c r="BS28" t="inlineStr"/>
+      <c r="BR28" t="inlineStr"/>
+      <c r="BS28" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
       <c r="BT28" t="inlineStr">
         <is>
-          <t>Daily</t>
+          <t>Highly portable</t>
         </is>
       </c>
       <c r="BU28" t="inlineStr">
         <is>
-          <t>Highly portable</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="BV28" t="inlineStr">
@@ -8352,39 +8368,35 @@
       </c>
       <c r="BW28" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>Always</t>
         </is>
       </c>
       <c r="BX28" t="inlineStr">
         <is>
-          <t>Always</t>
-        </is>
-      </c>
-      <c r="BY28" t="inlineStr">
-        <is>
           <t>Very safe</t>
         </is>
       </c>
-      <c r="BZ28" t="inlineStr"/>
-      <c r="CA28" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="BY28" t="inlineStr"/>
+      <c r="BZ28" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="CA28" t="inlineStr"/>
       <c r="CB28" t="inlineStr"/>
       <c r="CC28" t="inlineStr"/>
-      <c r="CD28" t="inlineStr"/>
-      <c r="CE28" t="inlineStr">
+      <c r="CD28" t="inlineStr">
         <is>
           <t>Urban</t>
         </is>
       </c>
-      <c r="CF28" t="inlineStr"/>
-      <c r="CG28" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="CE28" t="inlineStr"/>
+      <c r="CF28" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="CG28" t="inlineStr"/>
       <c r="CH28" t="inlineStr"/>
       <c r="CI28" t="inlineStr">
         <is>

</xml_diff>